<commit_message>
added negative shift condition. Still need to work out kinks tho
</commit_message>
<xml_diff>
--- a/experiment_no_shift/plan.xlsx
+++ b/experiment_no_shift/plan.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willclapp/Desktop/245B/Replication245B/experiment_no_shift/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8789FFDE-6BD6-404F-BABA-A510F9444BB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB75316-AA55-B74C-B1BA-A93C4C8C32CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="13660" windowHeight="20020"/>
+    <workbookView xWindow="17800" yWindow="460" windowWidth="13660" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plan" sheetId="1" r:id="rId1"/>
@@ -365,7 +365,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1199,11 +1199,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1628,8 +1628,8 @@
       <c r="A28">
         <v>6</v>
       </c>
-      <c r="B28">
-        <v>0</v>
+      <c r="B28" t="s">
+        <v>13</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1680,7 +1680,7 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1715,8 +1715,8 @@
       <c r="A34">
         <v>12</v>
       </c>
-      <c r="B34" t="s">
-        <v>14</v>
+      <c r="B34">
+        <v>0</v>
       </c>
       <c r="C34" t="s">
         <v>19</v>

</xml_diff>